<commit_message>
initial commit on retry-logic
</commit_message>
<xml_diff>
--- a/testData/loginData.xlsx
+++ b/testData/loginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhi1\IdeaProjects\automation-assignment\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43997732-2905-4772-B31A-23663AC708B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC1DDDC-439E-48AC-B6FA-259A5BE1342F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -33,13 +33,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>6j6nsf1hdz@mrotzis.com</t>
+    <t>payeba8662@baxima.com</t>
   </si>
   <si>
-    <t>pass1234</t>
-  </si>
-  <si>
-    <t>payeba8662@baxima.com</t>
+    <t>hicamod348@halbov.com</t>
   </si>
 </sst>
 </file>
@@ -360,7 +357,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -378,15 +375,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -395,6 +392,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{25FD6F48-039C-4DDF-A470-85F3240461B2}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{FFE0460E-EB67-4035-B834-0CE86D8AB837}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>